<commit_message>
new file:   Language distribution.png 	modified:   Language.csv 	modified:   draw_pie.py 	modified:   language.py 	modified:   language.xlsx
</commit_message>
<xml_diff>
--- a/language.xlsx
+++ b/language.xlsx
@@ -543,7 +543,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Language of Other Asian Countries</t>
+          <t>Languages of Other Asian Countries</t>
         </is>
       </c>
     </row>
@@ -566,7 +566,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Language of Other Asian Countries</t>
+          <t>Languages of Other Asian Countries</t>
         </is>
       </c>
     </row>
@@ -658,7 +658,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Language of Other Asian Countries</t>
+          <t>Languages of Other Asian Countries</t>
         </is>
       </c>
     </row>
@@ -704,7 +704,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Language of Other African Countries</t>
+          <t>Languages of Other African Countries</t>
         </is>
       </c>
     </row>
@@ -727,7 +727,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Language of Other European Countries</t>
+          <t>Languages of Other European Countries</t>
         </is>
       </c>
     </row>
@@ -750,7 +750,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Language of Other African Countries</t>
+          <t>Languages of Other African Countries</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Language of Other Asian Countries</t>
+          <t>Languages of Other Asian Countries</t>
         </is>
       </c>
     </row>
@@ -796,7 +796,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Language of Other European Countries</t>
+          <t>Languages of Other European Countries</t>
         </is>
       </c>
     </row>
@@ -819,7 +819,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Language of Other Asian Countries</t>
+          <t>Languages of Other Asian Countries</t>
         </is>
       </c>
     </row>
@@ -842,7 +842,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Language of Other Asian Countries</t>
+          <t>Languages of Other Asian Countries</t>
         </is>
       </c>
     </row>
@@ -865,7 +865,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Language of Other African Countries</t>
+          <t>Languages of Other African Countries</t>
         </is>
       </c>
     </row>
@@ -888,7 +888,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Language of Other European Countries</t>
+          <t>Languages of Other European Countries</t>
         </is>
       </c>
     </row>
@@ -934,7 +934,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Language of Other European Countries</t>
+          <t>Languages of Other European Countries</t>
         </is>
       </c>
     </row>
@@ -957,7 +957,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Language of Other Asian Countries</t>
+          <t>Languages of Other Asian Countries</t>
         </is>
       </c>
     </row>
@@ -980,7 +980,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Language of Other European Countries</t>
+          <t>Languages of Other European Countries</t>
         </is>
       </c>
     </row>
@@ -1003,7 +1003,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Language of Other European Countries</t>
+          <t>Languages of Other European Countries</t>
         </is>
       </c>
     </row>
@@ -1026,7 +1026,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Language of Other European Countries</t>
+          <t>Languages of Other European Countries</t>
         </is>
       </c>
     </row>
@@ -1049,7 +1049,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Language of Other European Countries</t>
+          <t>Languages of Other European Countries</t>
         </is>
       </c>
     </row>
@@ -1072,7 +1072,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Language of Other European Countries</t>
+          <t>Languages of Other European Countries</t>
         </is>
       </c>
     </row>
@@ -1095,7 +1095,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Language of Other European Countries</t>
+          <t>Languages of Other European Countries</t>
         </is>
       </c>
     </row>
@@ -1118,7 +1118,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Language of Other European Countries</t>
+          <t>Languages of Other European Countries</t>
         </is>
       </c>
     </row>
@@ -1141,7 +1141,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Language of Other European Countries</t>
+          <t>Languages of Other European Countries</t>
         </is>
       </c>
     </row>
@@ -1164,7 +1164,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Language of Other European Countries</t>
+          <t>Languages of Other European Countries</t>
         </is>
       </c>
     </row>
@@ -1187,7 +1187,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Language of Other European Countries</t>
+          <t>Languages of Other European Countries</t>
         </is>
       </c>
     </row>
@@ -1210,7 +1210,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Language of Other Asian Countries</t>
+          <t>Languages of Other Asian Countries</t>
         </is>
       </c>
     </row>
@@ -1233,7 +1233,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Language of Other European Countries</t>
+          <t>Languages of Other European Countries</t>
         </is>
       </c>
     </row>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Language of Other European Countries</t>
+          <t>Languages of Other European Countries</t>
         </is>
       </c>
     </row>
@@ -1279,7 +1279,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Language of Other European Countries</t>
+          <t>Languages of Other European Countries</t>
         </is>
       </c>
     </row>
@@ -1302,7 +1302,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Language of Other European Countries</t>
+          <t>Languages of Other European Countries</t>
         </is>
       </c>
     </row>
@@ -1325,7 +1325,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Language of Other European Countries</t>
+          <t>Languages of Other European Countries</t>
         </is>
       </c>
     </row>
@@ -1348,7 +1348,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Language of Other Asian Countries</t>
+          <t>Languages of Other Asian Countries</t>
         </is>
       </c>
     </row>
@@ -1371,7 +1371,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Language of Other European Countries</t>
+          <t>Languages of Other European Countries</t>
         </is>
       </c>
     </row>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Language of Other European Countries</t>
+          <t>Languages of Other European Countries</t>
         </is>
       </c>
     </row>
@@ -1417,7 +1417,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Language of Other Asian Countries</t>
+          <t>Languages of Other Asian Countries</t>
         </is>
       </c>
     </row>
@@ -1440,7 +1440,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Language of Other European Countries</t>
+          <t>Languages of Other European Countries</t>
         </is>
       </c>
     </row>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Language of Other Asian Countries</t>
+          <t>Languages of Other Asian Countries</t>
         </is>
       </c>
     </row>
@@ -1486,7 +1486,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Language of Other Asian Countries</t>
+          <t>Languages of Other Asian Countries</t>
         </is>
       </c>
     </row>
@@ -1509,7 +1509,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Language of Other European Countries</t>
+          <t>Languages of Other European Countries</t>
         </is>
       </c>
     </row>
@@ -1532,7 +1532,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Language of Other Asian Countries</t>
+          <t>Languages of Other Asian Countries</t>
         </is>
       </c>
     </row>
@@ -1555,7 +1555,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Language of Other Asian Countries</t>
+          <t>Languages of Other Asian Countries</t>
         </is>
       </c>
     </row>
@@ -1578,7 +1578,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Language of Other Asian Countries</t>
+          <t>Languages of Other Asian Countries</t>
         </is>
       </c>
     </row>
@@ -1601,7 +1601,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Language of Other Asian Countries</t>
+          <t>Languages of Other Asian Countries</t>
         </is>
       </c>
     </row>
@@ -1624,7 +1624,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Language of Other Asian Countries</t>
+          <t>Languages of Other Asian Countries</t>
         </is>
       </c>
     </row>
@@ -1647,7 +1647,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Language of Other European Countries</t>
+          <t>Languages of Other European Countries</t>
         </is>
       </c>
     </row>
@@ -1670,7 +1670,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Language of Other Asian Countries</t>
+          <t>Languages of Other Asian Countries</t>
         </is>
       </c>
     </row>
@@ -1693,7 +1693,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Language of Other Asian Countries</t>
+          <t>Languages of Other Asian Countries</t>
         </is>
       </c>
     </row>
@@ -1716,7 +1716,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Language of Other Asian Countries</t>
+          <t>Languages of Other Asian Countries</t>
         </is>
       </c>
     </row>
@@ -1739,7 +1739,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Language of Other Asian Countries</t>
+          <t>Languages of Other Asian Countries</t>
         </is>
       </c>
     </row>
@@ -1762,7 +1762,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Language of Other Asian Countries</t>
+          <t>Languages of Other Asian Countries</t>
         </is>
       </c>
     </row>
@@ -1785,7 +1785,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Language of Other Asian Countries</t>
+          <t>Languages of Other Asian Countries</t>
         </is>
       </c>
     </row>
@@ -1808,7 +1808,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Language of Other Asian Countries</t>
+          <t>Languages of Other Asian Countries</t>
         </is>
       </c>
     </row>

</xml_diff>